<commit_message>
changes for the ticket DCA-324 related to ccdi study tab.
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC01_CCDI_phs002504_Sex-Male.xlsx
+++ b/InputFiles/CCDI/TC01_CCDI_phs002504_Sex-Male.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-09-25-2024/Commons_Automation/InputFiles/CCDI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/radhakrishnang2/Desktop/Automation/February/Commons_Automation/InputFiles/CCDI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F6207A-D4F7-8543-93E0-EC7F515578C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC59644D-039C-4045-A90F-B31A456851F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-42460" yWindow="-2660" windowWidth="30240" windowHeight="25920" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="4680" yWindow="500" windowWidth="30240" windowHeight="19500" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -345,9 +344,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -428,14 +434,17 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -829,7 +838,7 @@
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="3"/>
@@ -860,7 +869,7 @@
       <c r="C8" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>